<commit_message>
add Results_Alex + edit final results
</commit_message>
<xml_diff>
--- a/project/results/Movie_Recommendations_Results.xlsx
+++ b/project/results/Movie_Recommendations_Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\Information Search and Recommendation Systems\recommender_systems_group4\project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5A042BD-203F-44BA-8168-4D92E87BE09A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68929BD7-05AF-4D86-9063-E05001E8049F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7A7E9DE-1054-4C8C-AE51-197445DE0130}"/>
+    <workbookView xWindow="31740" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{A7A7E9DE-1054-4C8C-AE51-197445DE0130}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98505350-CC81-44CF-9D4E-10B5295F0DFC}">
   <dimension ref="B8:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,10 +443,13 @@
       </c>
       <c r="C9">
         <f>(D9+E9+F9)/3</f>
-        <v>3.6166666666666667</v>
+        <v>5.416666666666667</v>
       </c>
       <c r="D9">
         <v>5.51</v>
+      </c>
+      <c r="E9">
+        <v>5.4</v>
       </c>
       <c r="F9">
         <v>5.34</v>
@@ -458,10 +461,13 @@
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C14" si="0">(D10+E10+F10)/3</f>
-        <v>4.123333333333334</v>
+        <v>6.1733333333333329</v>
       </c>
       <c r="D10">
         <v>6.23</v>
+      </c>
+      <c r="E10">
+        <v>6.15</v>
       </c>
       <c r="F10">
         <v>6.14</v>
@@ -472,8 +478,8 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>4.4933333333333332</v>
+        <f>(F11+D11)/2</f>
+        <v>6.74</v>
       </c>
       <c r="D11">
         <v>7.05</v>
@@ -488,10 +494,13 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>4.1166666666666663</v>
+        <v>6.1433333333333335</v>
       </c>
       <c r="D12">
         <v>5.96</v>
+      </c>
+      <c r="E12">
+        <v>6.08</v>
       </c>
       <c r="F12">
         <v>6.39</v>
@@ -503,10 +512,13 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>4.1000000000000005</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="D13">
         <v>6.27</v>
+      </c>
+      <c r="E13">
+        <v>6.2</v>
       </c>
       <c r="F13">
         <v>6.03</v>
@@ -518,10 +530,13 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>4.0866666666666669</v>
+        <v>6.0633333333333326</v>
       </c>
       <c r="D14">
         <v>6.02</v>
+      </c>
+      <c r="E14">
+        <v>5.93</v>
       </c>
       <c r="F14">
         <v>6.24</v>

</xml_diff>